<commit_message>
Latest version of question answer bank
</commit_message>
<xml_diff>
--- a/Angular-Question-Answer-DB.xlsx
+++ b/Angular-Question-Answer-DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jho/Documents/upskill-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7319812-24A7-3441-9D9F-E288DA8B1ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62132AF7-BCDB-4944-A243-8E1F998CD444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{80CEFDAA-1691-D444-858A-266A898A2367}"/>
+    <workbookView xWindow="14600" yWindow="760" windowWidth="15640" windowHeight="17440" xr2:uid="{80CEFDAA-1691-D444-858A-266A898A2367}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
   <si>
     <t>question_type</t>
   </si>
@@ -44,6 +44,340 @@
   </si>
   <si>
     <t>answer</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>OE</t>
+  </si>
+  <si>
+    <t>Which of the following is a recommended approach for handling asynchronous operations in Angular?
+a) Promises
+b) Observables
+c) Callbacks
+d) Async/Await</t>
+  </si>
+  <si>
+    <t>In Angular, what is the purpose of the @Input decorator?
+a) To declare a variable as an input property for a component
+b) To inject dependencies into a component
+c) To define a component's template
+d) To declare a variable as an output property for a component</t>
+  </si>
+  <si>
+    <t>Which of the following is a preferred method for handling form validation in Angular?
+a) Template-driven forms
+b) Reactive forms
+c) Both template-driven and reactive forms are equally preferred
+d) None of the above</t>
+  </si>
+  <si>
+    <t>What is the purpose of Angular's HttpClient module?
+a) To handle HTTP requests and responses
+b) To manage the state of an Angular application
+c) To provide routing functionality
+d) To handle animation effects</t>
+  </si>
+  <si>
+    <t>Which of the following is a recommended practice for optimizing Angular application performance?
+a) Minimizing the use of lazy loading
+b) Increasing bundle size to reduce the number of HTTP requests
+c) Employing AOT compilation
+d) Avoiding code splitting</t>
+  </si>
+  <si>
+    <t>What is the purpose of Angular's Dependency Injection (DI) system?
+a) To manage the application state
+b) To facilitate communication between components
+c) To inject dependencies into components, services, and other objects
+d) To define routing configurations</t>
+  </si>
+  <si>
+    <t>Which of the following is true about Angular's ngOnChanges lifecycle hook?
+a) It is called after ngOnInit hook
+b) It is called every time a component's input properties change
+c) It is used to initialize component properties
+d) It is called only once during component initialization</t>
+  </si>
+  <si>
+    <t>What is the purpose of the trackBy function in Angular's ngFor directive?
+a) To iterate over elements in an array
+b) To track changes in the DOM
+c) To improve performance by identifying unique items in a collection
+d) To define conditions for template rendering</t>
+  </si>
+  <si>
+    <t>Which of the following is a best practice for managing shared data and functionality in Angular?
+a) Using global variables
+b) Using the Singleton pattern
+c) Using Angular services
+d) Using local component state</t>
+  </si>
+  <si>
+    <t>What is the recommended way to handle routing in Angular applications?
+a) Using inline routing
+b) Using external routing libraries
+c) Using Angular's built-in RouterModule
+d) Using state management libraries like NgRx</t>
+  </si>
+  <si>
+    <t>Describe the purpose of Angular's NgModule and its role in organizing an Angular application.</t>
+  </si>
+  <si>
+    <t>Explain the difference between ViewChild and ContentChild in Angular and provide a scenario where each would be used.</t>
+  </si>
+  <si>
+    <t>Discuss the benefits of lazy loading modules in Angular and explain how it contributes to application performance.</t>
+  </si>
+  <si>
+    <t>Describe the role of the TestBed in Angular unit testing and explain how it is used to configure and execute tests.</t>
+  </si>
+  <si>
+    <t>What are Angular directives, and how do they differ from components? Provide examples of each.</t>
+  </si>
+  <si>
+    <t>Explain the concept of Angular's change detection mechanism and how it impacts application performance.</t>
+  </si>
+  <si>
+    <t>Describe the role of Angular services and provide examples of scenarios where services would be used in an application.</t>
+  </si>
+  <si>
+    <t>Discuss the advantages of using Angular's Ahead-of-Time (AOT) compilation over Just-in-Time (JIT) compilation.</t>
+  </si>
+  <si>
+    <t>Explain the purpose of Angular's HttpClientInterceptor and provide an example of how it can be used in an application.</t>
+  </si>
+  <si>
+    <t>Describe the process of internationalization and localization in Angular applications and discuss best practices for implementing multi-language support.</t>
+  </si>
+  <si>
+    <t>b) Observables</t>
+  </si>
+  <si>
+    <t>a) To declare a variable as an input property for a component</t>
+  </si>
+  <si>
+    <t>b) Reactive forms</t>
+  </si>
+  <si>
+    <t>a) To handle HTTP requests and responses</t>
+  </si>
+  <si>
+    <t>c) Employing AOT compilation</t>
+  </si>
+  <si>
+    <t>c) To inject dependencies into components, services, and other objects</t>
+  </si>
+  <si>
+    <t>b) It is called every time a component's input properties change</t>
+  </si>
+  <si>
+    <t>c) To improve performance by identifying unique items in a collection</t>
+  </si>
+  <si>
+    <t>c) Using Angular services</t>
+  </si>
+  <si>
+    <t>c) Using Angular's built-in RouterModule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NgModule in Angular is used to consolidate related components, directives, pipes, and services into cohesive blocks of functionality. It serves as a container for organizing and configuring the various elements that make up an Angular application. NgModule allows developers to define dependencies, declarations, providers, and other metadata necessary for Angular's compilation and runtime behavior.
+</t>
+  </si>
+  <si>
+    <t>ViewChild is used to access a child component, directive, or DOM element from a parent component's template. ContentChild, on the other hand, is used to access a directive or component that is projected into the parent component's view from the outside. ViewChild is typically used to interact with components or elements directly nested within the parent component, while ContentChild is used to interact with projected content.</t>
+  </si>
+  <si>
+    <t>Lazy loading modules in Angular allow developers to load modules asynchronously when they are needed, rather than loading them all at once when the application starts. This improves application startup time and reduces initial bundle size, leading to faster load times and better performance, especially for larger applications. Lazy loading is particularly beneficial for applications with multiple feature modules, as it allows for more efficient resource utilization and improves the overall user experience.</t>
+  </si>
+  <si>
+    <t>TestBed is a utility in Angular used for configuring and creating instances of components, services, and other Angular artifacts during unit testing. It provides a testing environment similar to Angular's dependency injection system, allowing developers to configure module dependencies, mock services, and perform assertions on component behavior. TestBed is essential for writing and executing unit tests in Angular applications, providing a clean and isolated environment for testing individual components and services.</t>
+  </si>
+  <si>
+    <t>Directives in Angular are instructions in the DOM that tell Angular to do something with a particular piece of DOM. They can be classified into three types: structural, attribute, and component. Structural directives like *ngIf and *ngFor manipulate the DOM by adding or removing elements based on conditions. Attribute directives like ngClass and ngStyle modify the appearance or behavior of elements. Components in Angular are directives with a template, representing reusable UI components that encapsulate logic and markup.</t>
+  </si>
+  <si>
+    <t>Angular's change detection mechanism is responsible for detecting and propagating changes made to the application's data model to the corresponding views. Angular uses a unidirectional data flow, where changes to the model trigger a process called change detection, which updates the view accordingly. Angular employs a zone-based change detection strategy, where change detection is triggered automatically by various events such as user interactions, asynchronous operations, or timer events. Change detection is a critical aspect of Angular's performance optimization, and developers must be mindful of its impact on application performance.</t>
+  </si>
+  <si>
+    <t>Angular services are singleton objects in Angular applications that are used to encapsulate and share data, business logic, or other common functionality across components. Services are injectable and can be provided at the module or component level, allowing them to be easily consumed by other parts of the application. Examples of scenarios where services would be used include data fetching from an API, performing authentication, caching data, or sharing state between components.</t>
+  </si>
+  <si>
+    <t>Ahead-of-Time (AOT) compilation in Angular is a build process that converts Angular application code into efficient JavaScript code during the build phase, before the application is deployed to production. AOT compilation offers several advantages over Just-in-Time (JIT) compilation, including improved application startup time, reduced bundle size, and better runtime performance. AOT-compiled code is optimized for production, with template and style optimizations, error checking at compile time, and elimination of unused code, resulting in faster rendering and better user experience.</t>
+  </si>
+  <si>
+    <t>HttpClientInterceptor in Angular is used to intercept HTTP requests and responses globally within an Angular application. It allows developers to modify requests or responses, add headers, handle errors, or perform other tasks before they are sent to the server or processed by the application. HttpClientInterceptor is implemented as a service in Angular and can be provided at the module level to intercept requests and responses across the entire application. It is commonly used for tasks such as adding authentication tokens, logging, caching, or handling API errors.</t>
+  </si>
+  <si>
+    <t>Internationalization (i18n) and localization (l10n) in Angular applications involve adapting the application to support multiple languages and cultural conventions. Angular provides built-in support for i18n and l10n through the @angular/localize package, allowing developers to internationalize text and localize formatting, dates, and numbers based on the user's locale. Best practices for implementing multi-language support in Angular include using Angular's i18n tools for extracting and managing translations, organizing translation files efficiently, and testing localized versions of the application to ensure proper functionality and user experience.</t>
+  </si>
+  <si>
+    <t>Which Angular feature is used to improve performance by preloading modules in the background?
+a) Lazy loading
+b) Ahead-of-Time (AOT) compilation
+c) Preloading strategy
+d) Dynamic component loading</t>
+  </si>
+  <si>
+    <t>What is the purpose of Angular's Renderer2 service?
+a) To handle HTTP requests and responses
+b) To manipulate the DOM directly
+c) To provide routing functionality
+d) To manage application state</t>
+  </si>
+  <si>
+    <t>In Angular, which lifecycle hook is used to perform cleanup tasks before a component is destroyed?
+a) ngOnInit
+b) ngOnDestroy
+c) ngOnChanges
+d) ngAfterViewInit</t>
+  </si>
+  <si>
+    <t>Which Angular feature is used to share data between a parent and its child components?
+a) Input properties
+b) Output properties
+c) ViewChild
+d) Dependency Injection</t>
+  </si>
+  <si>
+    <t>What is the purpose of Angular's ngZone service?
+a) To provide a zone for asynchronous operations
+b) To manage application state
+c) To handle routing navigation
+d) To create animations</t>
+  </si>
+  <si>
+    <t>Which of the following is a recommended approach for error handling in Angular HTTP requests?
+a) Using try-catch blocks
+b) Handling errors in the subscribe method
+c) Ignoring errors
+d) Handling errors in the component template</t>
+  </si>
+  <si>
+    <t>What is Angular's HttpClientTestingModule used for in unit testing?
+a) To mock HTTP requests and responses
+b) To test routing configurations
+c) To test Angular services
+d) To configure TestBed for component testing</t>
+  </si>
+  <si>
+    <t>Which Angular feature is used for animating elements and components?
+a) ngAnimate
+b) Angular Material
+c) Angular Animations
+d) CSS transitions</t>
+  </si>
+  <si>
+    <t>In Angular, which directive is used to add or remove CSS classes based on conditions?
+a) ngClass
+b) ngStyle
+c) ngIf
+d) ngFor</t>
+  </si>
+  <si>
+    <t>What is the purpose of Angular's ErrorHandler interface?
+a) To handle errors globally in an Angular application
+b) To define custom error messages
+c) To manage application routing
+d) To provide error logging functionality</t>
+  </si>
+  <si>
+    <t>Explain the concept of Angular's ViewEncapsulation and its role in styling components.</t>
+  </si>
+  <si>
+    <t>Describe the process of unit testing Angular components and services using TestBed and Jasmine.</t>
+  </si>
+  <si>
+    <t>Discuss the benefits of using Angular's Reactive Forms over Template-driven Forms, providing examples of scenarios where each would be appropriate.</t>
+  </si>
+  <si>
+    <t>Explain the purpose of Angular's ActivatedRoute service and provide an example of how it can be used to access route parameters.</t>
+  </si>
+  <si>
+    <t>Describe the concept of Angular's Dependency Injection (DI) and how it differs from traditional dependency management approaches.</t>
+  </si>
+  <si>
+    <t>Discuss the role of Angular's NgModule imports array and how it affects module dependencies and application structure.</t>
+  </si>
+  <si>
+    <t>Explain the concept of Angular's ContentProjection and how it is used to project content into component templates.</t>
+  </si>
+  <si>
+    <t>Describe the purpose of Angular's ViewChild and ContentChild decorators and provide examples of scenarios where each would be used.</t>
+  </si>
+  <si>
+    <t>Discuss the role of Angular's ChangeDetectorRef service in managing change detection and updating the view.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the purpose of Angular's HttpClientTestingModule and how it is used to mock HTTP requests in unit tests.
+</t>
+  </si>
+  <si>
+    <t>c) Preloading strategy</t>
+  </si>
+  <si>
+    <t>b) To manipulate the DOM directly</t>
+  </si>
+  <si>
+    <t>b) ngOnDestroy</t>
+  </si>
+  <si>
+    <t>a) Input properties</t>
+  </si>
+  <si>
+    <t>a) To provide a zone for asynchronous operations</t>
+  </si>
+  <si>
+    <t>b) Handling errors in the subscribe method</t>
+  </si>
+  <si>
+    <t>a) To mock HTTP requests and responses</t>
+  </si>
+  <si>
+    <t>c) Angular Animations</t>
+  </si>
+  <si>
+    <t>a) ngClass</t>
+  </si>
+  <si>
+    <t>a) To handle errors globally in an Angular application</t>
+  </si>
+  <si>
+    <t>ViewEncapsulation in Angular is used to encapsulate component styles and prevent them from leaking into other components or the global scope. It allows developers to define how component styles are applied and scoped by specifying one of three encapsulation options: Emulated, Native, or None. Emulated encapsulation is the default behavior, where Angular emulates shadow DOM behavior by adding unique attribute selectors to component styles. Native encapsulation uses native shadow DOM if available in the browser. None encapsulation disables encapsulation entirely, allowing component styles to affect the entire application.</t>
+  </si>
+  <si>
+    <t>Unit testing Angular components and services involves using TestBed to configure the testing environment and Jasmine for writing test specs and assertions. TestBed is used to create a testing module that provides dependencies and configurations required for testing components and services. Jasmine provides a test framework for writing descriptive test specs, organizing tests into suites, and defining expectations using matcher functions. Components and services are tested by creating instances of them within the TestBed environment and asserting expected behaviors and outcomes.</t>
+  </si>
+  <si>
+    <t>Reactive Forms in Angular provide a more robust and scalable approach to building forms compared to Template-driven Forms. Reactive Forms are preferred for complex forms with dynamic validation requirements and interactions. They are built programmatically using form controls and form groups, allowing for greater flexibility and control over form behavior. Template-driven Forms, on the other hand, are suitable for simpler forms with straightforward validation requirements. They are built using directives in the component template, making them easier to implement but less flexible for complex scenarios.</t>
+  </si>
+  <si>
+    <t>ActivatedRoute service in Angular is used to access route parameters, query parameters, and fragment identifiers associated with the current route. It provides information about the current route's path, parameters, data, and other properties. ActivatedRoute is commonly used in Angular components to retrieve route parameters dynamically and perform actions based on the current route state. For example, it can be used to extract route parameters from the URL and pass them as arguments to service methods or component functions.</t>
+  </si>
+  <si>
+    <t>Dependency Injection (DI) in Angular is a design pattern used to manage dependencies between objects by providing them externally rather than creating them internally. DI allows components, services, and other objects to be decoupled from their dependencies, making them more modular, reusable, and testable. Angular's DI system provides dependencies to components and services through constructor injection or property injection. This allows dependencies to be easily swapped or mocked during testing, facilitating unit testing and improving code maintainability.</t>
+  </si>
+  <si>
+    <t>The NgModule imports array in Angular is used to import other Angular modules into the current module, making their exported components, directives, pipes, and services available for use within the current module. It allows developers to compose applications from reusable and encapsulated modules, promoting modularity and code organization. Modules imported into the current module become part of the current module's dependency graph, affecting its compilation and runtime behavior. Importing modules into the NgModule imports array establishes module dependencies and determines the application's module hierarchy.</t>
+  </si>
+  <si>
+    <t>ContentProjection in Angular is a mechanism used to project content from a parent component into a child component's template. It allows developers to pass content, such as HTML markup or other Angular components, from the parent component's template to the child component's template. ContentProjection is achieved using Angular's ContentChild decorator, which allows the child component to select and access projected content within its template. This enables developers to create reusable and composable components that can accept and display dynamic content provided by their parent components.</t>
+  </si>
+  <si>
+    <t>ViewChild and ContentChild decorators in Angular are used to access child components, directives, or DOM elements from a parent component's template. ViewChild is used to access a single child component or DOM element, while ContentChild is used to access projected content within a child component's template. ViewChild is commonly used to interact with child components or elements directly nested within the parent component's template. ContentChild, on the other hand, is used to interact with projected content passed from the parent component into the child component's template using ContentProjection.'</t>
+  </si>
+  <si>
+    <t>ChangeDetectorRef service in Angular is used to manually trigger change detection and update the view when needed. It provides methods for marking components as dirty and scheduling change detection cycles. ChangeDetectorRef is commonly used in scenarios where changes to component data occur outside of Angular's normal change detection cycle, such as when working with asynchronous operations or integrating with third-party libraries. By using ChangeDetectorRef, developers can ensure that changes to component state are reflected in the view appropriately, maintaining the integrity of the application's UI.</t>
+  </si>
+  <si>
+    <t>HttpClientTestingModule in Angular is used for testing HTTP requests and responses in unit tests by providing mock implementations of HttpClient and HttpTestingController. It allows developers to simulate HTTP interactions within a controlled environment, without making actual network requests. HttpClientTestingModule provides methods for mocking HTTP responses, setting expectations for requests, and verifying that requests were made as expected. This enables developers to write unit tests for components and services that interact with HTTP services, ensuring that they behave correctly under various conditions.</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Angular</t>
   </si>
 </sst>
 </file>
@@ -79,8 +413,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,23 +732,591 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A697377-0CCE-A545-B214-C0B7D06C01DA}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="83.33203125" customWidth="1"/>
+    <col min="4" max="4" width="129" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>